<commit_message>
more testing and data translators
</commit_message>
<xml_diff>
--- a/data/published/2019_SealeCarlisleWetmoreFloweMickes/testInput.xlsx
+++ b/data/published/2019_SealeCarlisleWetmoreFloweMickes/testInput.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramickes/Google Drive/Current/18Modelling Programming/pyWitness/data/published/2019_Colloff_Flowe_Winsor_etal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauramickes/Google Drive/Current/18Modelling Programming/pyWitness/data/published/2019_SealeCarlisleWetmoreFloweMickes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8CF6F3-C73E-A841-BFE2-A9D70B91FCE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654CF673-59C0-2C44-B631-D972C8EADC4B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="1280" windowWidth="38960" windowHeight="22380" xr2:uid="{9ED41D21-AD87-EA4A-9860-FFB390C24F36}"/>
+    <workbookView xWindow="3380" yWindow="7100" windowWidth="38960" windowHeight="20800" xr2:uid="{9ED41D21-AD87-EA4A-9860-FFB390C24F36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="54">
   <si>
     <t>Data translator</t>
   </si>
@@ -186,19 +186,16 @@
     <t>pAUC</t>
   </si>
   <si>
-    <t>published_Colloff_Flowe_Winsor_2020()</t>
-  </si>
-  <si>
-    <t>ageGroup Young</t>
-  </si>
-  <si>
-    <t>ageGroup Middle</t>
-  </si>
-  <si>
-    <t>ageGroup Late</t>
-  </si>
-  <si>
-    <t>{"includeFinalSample":"yes"}</t>
+    <t>condition Simultaneous</t>
+  </si>
+  <si>
+    <t>condition Sequential</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>published_SealeCarlisle_Wetmore_Flowe_Mickes_2019_E1()</t>
   </si>
 </sst>
 </file>
@@ -576,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D299942-CAD7-8B42-80C6-6BA1FC3BDCD5}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -588,71 +585,51 @@
     <col min="2" max="7" width="20.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="19.5" style="1" customWidth="1"/>
     <col min="9" max="13" width="16.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5" style="1" customWidth="1"/>
-    <col min="15" max="19" width="16.83203125" style="1" customWidth="1"/>
-    <col min="20" max="16384" width="10.83203125" style="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -692,26 +669,8 @@
       <c r="M2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -751,144 +710,90 @@
       <c r="M3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="R5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -928,26 +833,8 @@
       <c r="M6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>34</v>
       </c>
@@ -987,26 +874,8 @@
       <c r="M7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="N7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1046,61 +915,43 @@
       <c r="M8" s="3">
         <v>2000</v>
       </c>
-      <c r="N8" s="3">
-        <v>2000</v>
-      </c>
-      <c r="O8" s="3">
-        <v>2000</v>
-      </c>
-      <c r="P8" s="3">
-        <v>2000</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>2000</v>
-      </c>
-      <c r="R8" s="3">
-        <v>2000</v>
-      </c>
-      <c r="S8" s="3">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>